<commit_message>
Finished data preparation and dashboard
</commit_message>
<xml_diff>
--- a/data/fall_2025.xlsx
+++ b/data/fall_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmedina\Documents\Projects\Colle_Park_Residential_Tree_Planting_PRogram\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CE7A34-2694-4C4E-BC39-57D454D36365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99012230-6C8F-42CF-B47D-32E8D4B3BB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1EA4D933-CDB0-4B84-97B4-D1BA82CABC2D}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Fall_2025!$A$1:$T$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Final list'!$A$1:$O$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Final list'!$A$1:$L$60</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2209" uniqueCount="796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2029" uniqueCount="748">
   <si>
     <t>City Dist</t>
   </si>
@@ -3001,138 +3001,6 @@
     <t>7307 Baylor Ave</t>
   </si>
   <si>
-    <t>301-356-0282</t>
-  </si>
-  <si>
-    <t>202-445-4361</t>
-  </si>
-  <si>
-    <t>608-556-9381</t>
-  </si>
-  <si>
-    <t>240-367-6069</t>
-  </si>
-  <si>
-    <t>831-233-4744</t>
-  </si>
-  <si>
-    <t>973-462-9755</t>
-  </si>
-  <si>
-    <t>917-539-9828</t>
-  </si>
-  <si>
-    <t>240-380-5733</t>
-  </si>
-  <si>
-    <t>585-794-9860</t>
-  </si>
-  <si>
-    <t>240-643-6648</t>
-  </si>
-  <si>
-    <t>202-425-2444</t>
-  </si>
-  <si>
-    <t>301-675-6905</t>
-  </si>
-  <si>
-    <t>240-601-9571</t>
-  </si>
-  <si>
-    <t>202-590-8994</t>
-  </si>
-  <si>
-    <t>301-395-0486</t>
-  </si>
-  <si>
-    <t>301-219-5790</t>
-  </si>
-  <si>
-    <t>202-316-8119</t>
-  </si>
-  <si>
-    <t>615-390-9660</t>
-  </si>
-  <si>
-    <t>831-430-6133</t>
-  </si>
-  <si>
-    <t>301-452-6220</t>
-  </si>
-  <si>
-    <t>301-775-6519</t>
-  </si>
-  <si>
-    <t>301-455-6134</t>
-  </si>
-  <si>
-    <t>302-824-5989</t>
-  </si>
-  <si>
-    <t>240-300-3187</t>
-  </si>
-  <si>
-    <t>248-953-1544</t>
-  </si>
-  <si>
-    <t>734-649-9987</t>
-  </si>
-  <si>
-    <t>610-737-1124</t>
-  </si>
-  <si>
-    <t>703-635-4396</t>
-  </si>
-  <si>
-    <t>202-446-3832</t>
-  </si>
-  <si>
-    <t>443-630-0054</t>
-  </si>
-  <si>
-    <t>240-350-1084</t>
-  </si>
-  <si>
-    <t>301-646-3537</t>
-  </si>
-  <si>
-    <t>240-030-5016</t>
-  </si>
-  <si>
-    <t>301-935-5041</t>
-  </si>
-  <si>
-    <t>703-677-7404</t>
-  </si>
-  <si>
-    <t>301-254-0239</t>
-  </si>
-  <si>
-    <t>301-537-3311</t>
-  </si>
-  <si>
-    <t>301-520-5720</t>
-  </si>
-  <si>
-    <t>240-644-4438</t>
-  </si>
-  <si>
-    <t>301-518-2052</t>
-  </si>
-  <si>
-    <t>301-906-1005</t>
-  </si>
-  <si>
-    <t>410-739-1112</t>
-  </si>
-  <si>
-    <t>347-261-3821</t>
-  </si>
-  <si>
-    <t>301-728-9983</t>
-  </si>
-  <si>
     <t>Emily Shohfi</t>
   </si>
   <si>
@@ -3152,18 +3020,6 @@
   </si>
   <si>
     <t>7400 Dartmouth Ave</t>
-  </si>
-  <si>
-    <t>301-526-6660</t>
-  </si>
-  <si>
-    <t>202-246-3979</t>
-  </si>
-  <si>
-    <t>610-306-4219</t>
-  </si>
-  <si>
-    <t>301-742-4442</t>
   </si>
   <si>
     <t>Address</t>
@@ -4401,12 +4257,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{7E26C4FE-803A-4D0D-AD17-9A8152A95EDA}" name="Table10" displayName="Table10" ref="A1:H60" totalsRowShown="0">
-  <autoFilter ref="A1:H60" xr:uid="{7E26C4FE-803A-4D0D-AD17-9A8152A95EDA}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{184A32B1-C49F-48B4-9349-4BC42DB2194F}" name="First and Last Name:"/>
-    <tableColumn id="2" xr3:uid="{13E365B7-D254-4A12-91B7-A00896A41C90}" name="Email Address:"/>
-    <tableColumn id="3" xr3:uid="{FEABE689-AD64-496C-8F1F-A0679349ACA9}" name="Phone Number:"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{7E26C4FE-803A-4D0D-AD17-9A8152A95EDA}" name="Table10" displayName="Table10" ref="A1:E60" totalsRowShown="0">
+  <autoFilter ref="A1:E60" xr:uid="{7E26C4FE-803A-4D0D-AD17-9A8152A95EDA}"/>
+  <tableColumns count="5">
     <tableColumn id="4" xr3:uid="{9002049D-E1C9-4ABB-A47C-3BB495D2BD75}" name="District"/>
     <tableColumn id="5" xr3:uid="{CB90C922-0C8F-4D57-80DD-2B2BBBB26157}" name="Address"/>
     <tableColumn id="6" xr3:uid="{B681F585-CC8B-4CD5-AF26-562DF2B63DA4}" name="Species 1"/>
@@ -4857,1487 +4710,944 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B1" t="s">
+        <v>747</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>255</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>412</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>293</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>414</v>
+      </c>
+      <c r="B4" t="s">
+        <v>366</v>
+      </c>
+      <c r="C4" t="s">
+        <v>254</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>413</v>
+      </c>
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" t="s">
+        <v>317</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>412</v>
+      </c>
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
+        <v>292</v>
+      </c>
+      <c r="D6" t="s">
+        <v>304</v>
+      </c>
+      <c r="E6">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>411</v>
-      </c>
-      <c r="E1" t="s">
-        <v>795</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" t="s">
-        <v>740</v>
-      </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>412</v>
       </c>
-      <c r="E2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="B7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" t="s">
+        <v>292</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>414</v>
+      </c>
+      <c r="B8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" t="s">
+        <v>293</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>414</v>
+      </c>
+      <c r="B9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" t="s">
+        <v>318</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>412</v>
+      </c>
+      <c r="B10" t="s">
+        <v>334</v>
+      </c>
+      <c r="C10" t="s">
+        <v>309</v>
+      </c>
+      <c r="D10" t="s">
+        <v>254</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>412</v>
+      </c>
+      <c r="B11" t="s">
+        <v>337</v>
+      </c>
+      <c r="C11" t="s">
+        <v>310</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>412</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>316</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>412</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s">
+        <v>268</v>
+      </c>
+      <c r="D13" t="s">
+        <v>307</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>414</v>
+      </c>
+      <c r="B14" t="s">
+        <v>406</v>
+      </c>
+      <c r="C14" t="s">
+        <v>294</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>414</v>
+      </c>
+      <c r="B15" t="s">
+        <v>420</v>
+      </c>
+      <c r="C15" t="s">
+        <v>311</v>
+      </c>
+      <c r="D15" t="s">
+        <v>309</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>412</v>
+      </c>
+      <c r="B16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" t="s">
+        <v>309</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>412</v>
+      </c>
+      <c r="B17" t="s">
+        <v>346</v>
+      </c>
+      <c r="C17" t="s">
+        <v>309</v>
+      </c>
+      <c r="D17" t="s">
         <v>255</v>
       </c>
-      <c r="H2">
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>412</v>
+      </c>
+      <c r="B18" t="s">
+        <v>261</v>
+      </c>
+      <c r="C18" t="s">
+        <v>309</v>
+      </c>
+      <c r="D18" t="s">
+        <v>306</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>414</v>
+      </c>
+      <c r="B19" t="s">
+        <v>253</v>
+      </c>
+      <c r="C19" t="s">
+        <v>292</v>
+      </c>
+      <c r="E19">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" t="s">
-        <v>741</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>412</v>
       </c>
-      <c r="E3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="B20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" t="s">
+        <v>306</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>414</v>
+      </c>
+      <c r="B21" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" t="s">
+        <v>305</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>414</v>
+      </c>
+      <c r="B22" t="s">
+        <v>352</v>
+      </c>
+      <c r="C22" t="s">
+        <v>254</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>413</v>
+      </c>
+      <c r="B23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" t="s">
+        <v>314</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>415</v>
+      </c>
+      <c r="B24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" t="s">
+        <v>255</v>
+      </c>
+      <c r="D24" t="s">
+        <v>311</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>414</v>
+      </c>
+      <c r="B25" t="s">
+        <v>379</v>
+      </c>
+      <c r="C25" t="s">
+        <v>306</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>415</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s">
+        <v>295</v>
+      </c>
+      <c r="D26" t="s">
+        <v>255</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>412</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
         <v>293</v>
       </c>
-      <c r="H3">
+      <c r="E27">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>364</v>
-      </c>
-      <c r="B4" t="s">
-        <v>365</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>412</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>268</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>412</v>
+      </c>
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" t="s">
+        <v>294</v>
+      </c>
+      <c r="D29" t="s">
+        <v>295</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>412</v>
+      </c>
+      <c r="B30" t="s">
+        <v>392</v>
+      </c>
+      <c r="C30" t="s">
+        <v>304</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>414</v>
+      </c>
+      <c r="B31" t="s">
+        <v>389</v>
+      </c>
+      <c r="C31" t="s">
+        <v>292</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>412</v>
+      </c>
+      <c r="B32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" t="s">
+        <v>294</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>412</v>
+      </c>
+      <c r="B33" t="s">
+        <v>407</v>
+      </c>
+      <c r="C33" t="s">
+        <v>317</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>412</v>
+      </c>
+      <c r="B34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" t="s">
+        <v>316</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>413</v>
+      </c>
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" t="s">
+        <v>295</v>
+      </c>
+      <c r="D35" t="s">
+        <v>293</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>414</v>
+      </c>
+      <c r="B36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" t="s">
+        <v>309</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>414</v>
+      </c>
+      <c r="B37" t="s">
+        <v>355</v>
+      </c>
+      <c r="C37" t="s">
+        <v>295</v>
+      </c>
+      <c r="D37" t="s">
+        <v>304</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>413</v>
+      </c>
+      <c r="B38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" t="s">
+        <v>268</v>
+      </c>
+      <c r="D38" t="s">
+        <v>317</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>412</v>
+      </c>
+      <c r="B39" t="s">
+        <v>264</v>
+      </c>
+      <c r="C39" t="s">
+        <v>294</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>412</v>
+      </c>
+      <c r="B40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" t="s">
+        <v>293</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>415</v>
+      </c>
+      <c r="B41" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" t="s">
+        <v>293</v>
+      </c>
+      <c r="D41" t="s">
+        <v>293</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>415</v>
+      </c>
+      <c r="B42" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" t="s">
+        <v>255</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>412</v>
+      </c>
+      <c r="B43" t="s">
+        <v>398</v>
+      </c>
+      <c r="C43" t="s">
+        <v>306</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>414</v>
+      </c>
+      <c r="B44" t="s">
+        <v>408</v>
+      </c>
+      <c r="C44" t="s">
+        <v>292</v>
+      </c>
+      <c r="D44" t="s">
+        <v>303</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>412</v>
+      </c>
+      <c r="B45" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45" t="s">
+        <v>303</v>
+      </c>
+      <c r="D45" t="s">
+        <v>303</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>412</v>
+      </c>
+      <c r="B46" t="s">
+        <v>331</v>
+      </c>
+      <c r="C46" t="s">
+        <v>303</v>
+      </c>
+      <c r="D46" t="s">
+        <v>254</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>413</v>
+      </c>
+      <c r="B47" t="s">
+        <v>361</v>
+      </c>
+      <c r="C47" t="s">
+        <v>311</v>
+      </c>
+      <c r="D47" t="s">
+        <v>294</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>412</v>
+      </c>
+      <c r="B48" t="s">
+        <v>91</v>
+      </c>
+      <c r="C48" t="s">
+        <v>317</v>
+      </c>
+      <c r="D48" t="s">
+        <v>304</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>413</v>
+      </c>
+      <c r="B49" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" t="s">
+        <v>324</v>
+      </c>
+      <c r="D49" t="s">
+        <v>316</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>412</v>
+      </c>
+      <c r="B50" t="s">
+        <v>92</v>
+      </c>
+      <c r="C50" t="s">
+        <v>255</v>
+      </c>
+      <c r="D50" t="s">
+        <v>254</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>412</v>
+      </c>
+      <c r="B51" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" t="s">
+        <v>293</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>412</v>
+      </c>
+      <c r="B52" t="s">
+        <v>394</v>
+      </c>
+      <c r="C52" t="s">
+        <v>294</v>
+      </c>
+      <c r="D52" t="s">
+        <v>254</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>415</v>
+      </c>
+      <c r="B53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C53" t="s">
+        <v>268</v>
+      </c>
+      <c r="D53" t="s">
+        <v>309</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>412</v>
+      </c>
+      <c r="B54" t="s">
+        <v>731</v>
+      </c>
+      <c r="C54" t="s">
+        <v>303</v>
+      </c>
+      <c r="D54" t="s">
+        <v>311</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>412</v>
+      </c>
+      <c r="B55" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55" t="s">
+        <v>318</v>
+      </c>
+      <c r="D55" t="s">
+        <v>318</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>415</v>
+      </c>
+      <c r="B56" t="s">
+        <v>36</v>
+      </c>
+      <c r="C56" t="s">
+        <v>303</v>
+      </c>
+      <c r="D56" t="s">
+        <v>255</v>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>414</v>
+      </c>
+      <c r="B57" t="s">
+        <v>383</v>
+      </c>
+      <c r="C57" t="s">
+        <v>303</v>
+      </c>
+      <c r="D57" t="s">
+        <v>303</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>414</v>
+      </c>
+      <c r="B58" t="s">
+        <v>739</v>
+      </c>
+      <c r="C58" t="s">
+        <v>294</v>
+      </c>
+      <c r="D58" t="s">
+        <v>307</v>
+      </c>
+      <c r="E58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>413</v>
+      </c>
+      <c r="B59" t="s">
         <v>742</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C59" t="s">
+        <v>743</v>
+      </c>
+      <c r="D59" t="s">
+        <v>743</v>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>414</v>
       </c>
-      <c r="E4" t="s">
-        <v>366</v>
-      </c>
-      <c r="F4" t="s">
-        <v>254</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" t="s">
-        <v>247</v>
-      </c>
-      <c r="D5" t="s">
-        <v>413</v>
-      </c>
-      <c r="E5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F5" t="s">
-        <v>317</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" t="s">
-        <v>743</v>
-      </c>
-      <c r="D6" t="s">
-        <v>412</v>
-      </c>
-      <c r="E6" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" t="s">
-        <v>292</v>
-      </c>
-      <c r="G6" t="s">
-        <v>304</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7" t="s">
-        <v>122</v>
-      </c>
-      <c r="C7" t="s">
-        <v>249</v>
-      </c>
-      <c r="D7" t="s">
-        <v>412</v>
-      </c>
-      <c r="E7" t="s">
-        <v>104</v>
-      </c>
-      <c r="F7" t="s">
-        <v>292</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B8" t="s">
-        <v>124</v>
-      </c>
-      <c r="C8" t="s">
-        <v>744</v>
-      </c>
-      <c r="D8" t="s">
-        <v>414</v>
-      </c>
-      <c r="E8" t="s">
-        <v>103</v>
-      </c>
-      <c r="F8" t="s">
-        <v>293</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" t="s">
-        <v>107</v>
-      </c>
-      <c r="C9" t="s">
-        <v>745</v>
-      </c>
-      <c r="D9" t="s">
-        <v>414</v>
-      </c>
-      <c r="E9" t="s">
-        <v>98</v>
-      </c>
-      <c r="F9" t="s">
-        <v>318</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>332</v>
-      </c>
-      <c r="B10" t="s">
-        <v>333</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B60" t="s">
         <v>746</v>
       </c>
-      <c r="D10" t="s">
-        <v>412</v>
-      </c>
-      <c r="E10" t="s">
-        <v>334</v>
-      </c>
-      <c r="F10" t="s">
-        <v>309</v>
-      </c>
-      <c r="G10" t="s">
-        <v>254</v>
-      </c>
-      <c r="H10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>335</v>
-      </c>
-      <c r="B11" t="s">
-        <v>336</v>
-      </c>
-      <c r="C11" t="s">
-        <v>747</v>
-      </c>
-      <c r="D11" t="s">
-        <v>412</v>
-      </c>
-      <c r="E11" t="s">
-        <v>337</v>
-      </c>
-      <c r="F11" t="s">
-        <v>310</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>748</v>
-      </c>
-      <c r="D12" t="s">
-        <v>412</v>
-      </c>
-      <c r="E12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" t="s">
-        <v>316</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" t="s">
-        <v>749</v>
-      </c>
-      <c r="D13" t="s">
-        <v>412</v>
-      </c>
-      <c r="E13" t="s">
-        <v>62</v>
-      </c>
-      <c r="F13" t="s">
-        <v>268</v>
-      </c>
-      <c r="G13" t="s">
-        <v>307</v>
-      </c>
-      <c r="H13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>404</v>
-      </c>
-      <c r="B14" t="s">
-        <v>405</v>
-      </c>
-      <c r="C14" t="s">
-        <v>750</v>
-      </c>
-      <c r="D14" t="s">
-        <v>414</v>
-      </c>
-      <c r="E14" t="s">
-        <v>406</v>
-      </c>
-      <c r="F14" t="s">
-        <v>294</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>89</v>
-      </c>
-      <c r="B15" t="s">
-        <v>123</v>
-      </c>
-      <c r="C15" t="s">
-        <v>751</v>
-      </c>
-      <c r="D15" t="s">
-        <v>414</v>
-      </c>
-      <c r="E15" t="s">
-        <v>420</v>
-      </c>
-      <c r="F15" t="s">
-        <v>311</v>
-      </c>
-      <c r="G15" t="s">
-        <v>309</v>
-      </c>
-      <c r="H15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B16" t="s">
-        <v>108</v>
-      </c>
-      <c r="C16" t="s">
-        <v>233</v>
-      </c>
-      <c r="D16" t="s">
-        <v>412</v>
-      </c>
-      <c r="E16" t="s">
-        <v>96</v>
-      </c>
-      <c r="F16" t="s">
-        <v>309</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>344</v>
-      </c>
-      <c r="B17" t="s">
-        <v>345</v>
-      </c>
-      <c r="C17" t="s">
-        <v>752</v>
-      </c>
-      <c r="D17" t="s">
-        <v>412</v>
-      </c>
-      <c r="E17" t="s">
-        <v>346</v>
-      </c>
-      <c r="F17" t="s">
-        <v>309</v>
-      </c>
-      <c r="G17" t="s">
-        <v>255</v>
-      </c>
-      <c r="H17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>362</v>
-      </c>
-      <c r="B18" t="s">
-        <v>260</v>
-      </c>
-      <c r="C18" t="s">
-        <v>753</v>
-      </c>
-      <c r="D18" t="s">
-        <v>412</v>
-      </c>
-      <c r="E18" t="s">
-        <v>261</v>
-      </c>
-      <c r="F18" t="s">
-        <v>309</v>
-      </c>
-      <c r="G18" t="s">
-        <v>306</v>
-      </c>
-      <c r="H18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" t="s">
-        <v>209</v>
-      </c>
-      <c r="D19" t="s">
-        <v>414</v>
-      </c>
-      <c r="E19" t="s">
-        <v>253</v>
-      </c>
-      <c r="F19" t="s">
-        <v>292</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" t="s">
-        <v>754</v>
-      </c>
-      <c r="D20" t="s">
-        <v>412</v>
-      </c>
-      <c r="E20" t="s">
-        <v>65</v>
-      </c>
-      <c r="F20" t="s">
-        <v>306</v>
-      </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>84</v>
-      </c>
-      <c r="B21" t="s">
-        <v>117</v>
-      </c>
-      <c r="C21" t="s">
-        <v>755</v>
-      </c>
-      <c r="D21" t="s">
-        <v>414</v>
-      </c>
-      <c r="E21" t="s">
-        <v>106</v>
-      </c>
-      <c r="F21" t="s">
-        <v>305</v>
-      </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>350</v>
-      </c>
-      <c r="B22" t="s">
-        <v>351</v>
-      </c>
-      <c r="C22" t="s">
-        <v>756</v>
-      </c>
-      <c r="D22" t="s">
-        <v>414</v>
-      </c>
-      <c r="E22" t="s">
-        <v>352</v>
-      </c>
-      <c r="F22" t="s">
-        <v>254</v>
-      </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>85</v>
-      </c>
-      <c r="B23" t="s">
-        <v>118</v>
-      </c>
-      <c r="C23" t="s">
-        <v>757</v>
-      </c>
-      <c r="D23" t="s">
-        <v>413</v>
-      </c>
-      <c r="E23" t="s">
-        <v>94</v>
-      </c>
-      <c r="F23" t="s">
-        <v>314</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" t="s">
-        <v>112</v>
-      </c>
-      <c r="C24" t="s">
-        <v>758</v>
-      </c>
-      <c r="D24" t="s">
-        <v>415</v>
-      </c>
-      <c r="E24" t="s">
-        <v>99</v>
-      </c>
-      <c r="F24" t="s">
-        <v>255</v>
-      </c>
-      <c r="G24" t="s">
-        <v>311</v>
-      </c>
-      <c r="H24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>377</v>
-      </c>
-      <c r="B25" t="s">
-        <v>378</v>
-      </c>
-      <c r="C25" t="s">
-        <v>759</v>
-      </c>
-      <c r="D25" t="s">
-        <v>414</v>
-      </c>
-      <c r="E25" t="s">
-        <v>379</v>
-      </c>
-      <c r="F25" t="s">
-        <v>306</v>
-      </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" t="s">
-        <v>119</v>
-      </c>
-      <c r="C26" t="s">
-        <v>760</v>
-      </c>
-      <c r="D26" t="s">
-        <v>415</v>
-      </c>
-      <c r="E26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" t="s">
-        <v>295</v>
-      </c>
-      <c r="G26" t="s">
-        <v>255</v>
-      </c>
-      <c r="H26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" t="s">
-        <v>761</v>
-      </c>
-      <c r="D27" t="s">
-        <v>412</v>
-      </c>
-      <c r="E27" t="s">
-        <v>29</v>
-      </c>
-      <c r="F27" t="s">
-        <v>293</v>
-      </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" t="s">
-        <v>762</v>
-      </c>
-      <c r="D28" t="s">
-        <v>412</v>
-      </c>
-      <c r="E28" t="s">
-        <v>27</v>
-      </c>
-      <c r="F28" t="s">
-        <v>268</v>
-      </c>
-      <c r="H28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B29" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" t="s">
-        <v>230</v>
-      </c>
-      <c r="D29" t="s">
-        <v>412</v>
-      </c>
-      <c r="E29" t="s">
-        <v>68</v>
-      </c>
-      <c r="F29" t="s">
-        <v>294</v>
-      </c>
-      <c r="G29" t="s">
-        <v>295</v>
-      </c>
-      <c r="H29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>390</v>
-      </c>
-      <c r="B30" t="s">
-        <v>391</v>
-      </c>
-      <c r="C30" t="s">
-        <v>763</v>
-      </c>
-      <c r="D30" t="s">
-        <v>412</v>
-      </c>
-      <c r="E30" t="s">
-        <v>392</v>
-      </c>
-      <c r="F30" t="s">
-        <v>304</v>
-      </c>
-      <c r="H30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>387</v>
-      </c>
-      <c r="B31" t="s">
-        <v>388</v>
-      </c>
-      <c r="C31" t="s">
-        <v>764</v>
-      </c>
-      <c r="D31" t="s">
-        <v>414</v>
-      </c>
-      <c r="E31" t="s">
-        <v>389</v>
-      </c>
-      <c r="F31" t="s">
-        <v>292</v>
-      </c>
-      <c r="H31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32" t="s">
-        <v>72</v>
-      </c>
-      <c r="C32" t="s">
-        <v>765</v>
-      </c>
-      <c r="D32" t="s">
-        <v>412</v>
-      </c>
-      <c r="E32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F32" t="s">
-        <v>294</v>
-      </c>
-      <c r="H32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>297</v>
-      </c>
-      <c r="B33" t="s">
-        <v>298</v>
-      </c>
-      <c r="C33" t="s">
-        <v>766</v>
-      </c>
-      <c r="D33" t="s">
-        <v>412</v>
-      </c>
-      <c r="E33" t="s">
-        <v>407</v>
-      </c>
-      <c r="F33" t="s">
-        <v>317</v>
-      </c>
-      <c r="H33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>69</v>
-      </c>
-      <c r="B34" t="s">
-        <v>125</v>
-      </c>
-      <c r="C34" t="s">
-        <v>767</v>
-      </c>
-      <c r="D34" t="s">
-        <v>412</v>
-      </c>
-      <c r="E34" t="s">
-        <v>70</v>
-      </c>
-      <c r="F34" t="s">
-        <v>316</v>
-      </c>
-      <c r="H34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>8</v>
-      </c>
-      <c r="B35" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" t="s">
-        <v>204</v>
-      </c>
-      <c r="D35" t="s">
-        <v>413</v>
-      </c>
-      <c r="E35" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35" t="s">
-        <v>295</v>
-      </c>
-      <c r="G35" t="s">
-        <v>293</v>
-      </c>
-      <c r="H35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>82</v>
-      </c>
-      <c r="B36" t="s">
-        <v>115</v>
-      </c>
-      <c r="C36" t="s">
-        <v>768</v>
-      </c>
-      <c r="D36" t="s">
-        <v>414</v>
-      </c>
-      <c r="E36" t="s">
-        <v>102</v>
-      </c>
-      <c r="F36" t="s">
-        <v>309</v>
-      </c>
-      <c r="H36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>353</v>
-      </c>
-      <c r="B37" t="s">
-        <v>354</v>
-      </c>
-      <c r="C37" t="s">
-        <v>769</v>
-      </c>
-      <c r="D37" t="s">
-        <v>414</v>
-      </c>
-      <c r="E37" t="s">
-        <v>355</v>
-      </c>
-      <c r="F37" t="s">
-        <v>295</v>
-      </c>
-      <c r="G37" t="s">
-        <v>304</v>
-      </c>
-      <c r="H37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>22</v>
-      </c>
-      <c r="B38" t="s">
-        <v>23</v>
-      </c>
-      <c r="C38" t="s">
-        <v>770</v>
-      </c>
-      <c r="D38" t="s">
-        <v>413</v>
-      </c>
-      <c r="E38" t="s">
-        <v>24</v>
-      </c>
-      <c r="F38" t="s">
-        <v>268</v>
-      </c>
-      <c r="G38" t="s">
-        <v>317</v>
-      </c>
-      <c r="H38">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>262</v>
-      </c>
-      <c r="B39" t="s">
-        <v>263</v>
-      </c>
-      <c r="C39" t="s">
-        <v>771</v>
-      </c>
-      <c r="D39" t="s">
-        <v>412</v>
-      </c>
-      <c r="E39" t="s">
-        <v>264</v>
-      </c>
-      <c r="F39" t="s">
-        <v>294</v>
-      </c>
-      <c r="H39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>48</v>
-      </c>
-      <c r="B40" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40" t="s">
-        <v>772</v>
-      </c>
-      <c r="D40" t="s">
-        <v>412</v>
-      </c>
-      <c r="E40" t="s">
-        <v>50</v>
-      </c>
-      <c r="F40" t="s">
-        <v>293</v>
-      </c>
-      <c r="H40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>220</v>
-      </c>
-      <c r="B41" t="s">
-        <v>43</v>
-      </c>
-      <c r="C41" t="s">
-        <v>222</v>
-      </c>
-      <c r="D41" t="s">
-        <v>415</v>
-      </c>
-      <c r="E41" t="s">
-        <v>44</v>
-      </c>
-      <c r="F41" t="s">
-        <v>293</v>
-      </c>
-      <c r="G41" t="s">
-        <v>293</v>
-      </c>
-      <c r="H41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>80</v>
-      </c>
-      <c r="B42" t="s">
-        <v>113</v>
-      </c>
-      <c r="C42" t="s">
-        <v>773</v>
-      </c>
-      <c r="D42" t="s">
-        <v>415</v>
-      </c>
-      <c r="E42" t="s">
-        <v>100</v>
-      </c>
-      <c r="F42" t="s">
-        <v>255</v>
-      </c>
-      <c r="H42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>396</v>
-      </c>
-      <c r="B43" t="s">
-        <v>397</v>
-      </c>
-      <c r="C43" t="s">
-        <v>774</v>
-      </c>
-      <c r="D43" t="s">
-        <v>412</v>
-      </c>
-      <c r="E43" t="s">
-        <v>398</v>
-      </c>
-      <c r="F43" t="s">
-        <v>306</v>
-      </c>
-      <c r="H43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>373</v>
-      </c>
-      <c r="B44" t="s">
-        <v>380</v>
-      </c>
-      <c r="C44" t="s">
-        <v>775</v>
-      </c>
-      <c r="D44" t="s">
-        <v>414</v>
-      </c>
-      <c r="E44" t="s">
-        <v>408</v>
-      </c>
-      <c r="F44" t="s">
-        <v>292</v>
-      </c>
-      <c r="G44" t="s">
-        <v>303</v>
-      </c>
-      <c r="H44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>51</v>
-      </c>
-      <c r="B45" t="s">
-        <v>52</v>
-      </c>
-      <c r="C45" t="s">
-        <v>226</v>
-      </c>
-      <c r="D45" t="s">
-        <v>412</v>
-      </c>
-      <c r="E45" t="s">
-        <v>53</v>
-      </c>
-      <c r="F45" t="s">
-        <v>303</v>
-      </c>
-      <c r="G45" t="s">
-        <v>303</v>
-      </c>
-      <c r="H45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>329</v>
-      </c>
-      <c r="B46" t="s">
-        <v>330</v>
-      </c>
-      <c r="C46" t="s">
-        <v>776</v>
-      </c>
-      <c r="D46" t="s">
-        <v>412</v>
-      </c>
-      <c r="E46" t="s">
-        <v>331</v>
-      </c>
-      <c r="F46" t="s">
-        <v>303</v>
-      </c>
-      <c r="G46" t="s">
-        <v>254</v>
-      </c>
-      <c r="H46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>359</v>
-      </c>
-      <c r="B47" t="s">
-        <v>360</v>
-      </c>
-      <c r="C47" t="s">
-        <v>777</v>
-      </c>
-      <c r="D47" t="s">
-        <v>413</v>
-      </c>
-      <c r="E47" t="s">
-        <v>361</v>
-      </c>
-      <c r="F47" t="s">
-        <v>311</v>
-      </c>
-      <c r="G47" t="s">
-        <v>294</v>
-      </c>
-      <c r="H47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>76</v>
-      </c>
-      <c r="B48" t="s">
-        <v>109</v>
-      </c>
-      <c r="C48" t="s">
-        <v>778</v>
-      </c>
-      <c r="D48" t="s">
-        <v>412</v>
-      </c>
-      <c r="E48" t="s">
-        <v>91</v>
-      </c>
-      <c r="F48" t="s">
-        <v>317</v>
-      </c>
-      <c r="G48" t="s">
-        <v>304</v>
-      </c>
-      <c r="H48">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>81</v>
-      </c>
-      <c r="B49" t="s">
-        <v>114</v>
-      </c>
-      <c r="C49" t="s">
-        <v>241</v>
-      </c>
-      <c r="D49" t="s">
-        <v>413</v>
-      </c>
-      <c r="E49" t="s">
-        <v>101</v>
-      </c>
-      <c r="F49" t="s">
+      <c r="C60" t="s">
         <v>324</v>
       </c>
-      <c r="G49" t="s">
-        <v>316</v>
-      </c>
-      <c r="H49">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>77</v>
-      </c>
-      <c r="B50" t="s">
-        <v>110</v>
-      </c>
-      <c r="C50" t="s">
-        <v>779</v>
-      </c>
-      <c r="D50" t="s">
-        <v>412</v>
-      </c>
-      <c r="E50" t="s">
-        <v>92</v>
-      </c>
-      <c r="F50" t="s">
-        <v>255</v>
-      </c>
-      <c r="G50" t="s">
-        <v>254</v>
-      </c>
-      <c r="H50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>78</v>
-      </c>
-      <c r="B51" t="s">
-        <v>111</v>
-      </c>
-      <c r="C51" t="s">
-        <v>235</v>
-      </c>
-      <c r="D51" t="s">
-        <v>412</v>
-      </c>
-      <c r="E51" t="s">
-        <v>97</v>
-      </c>
-      <c r="F51" t="s">
-        <v>293</v>
-      </c>
-      <c r="H51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>393</v>
-      </c>
-      <c r="B52" t="s">
-        <v>395</v>
-      </c>
-      <c r="C52" t="s">
-        <v>780</v>
-      </c>
-      <c r="D52" t="s">
-        <v>412</v>
-      </c>
-      <c r="E52" t="s">
-        <v>394</v>
-      </c>
-      <c r="F52" t="s">
-        <v>294</v>
-      </c>
-      <c r="G52" t="s">
-        <v>254</v>
-      </c>
-      <c r="H52">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>86</v>
-      </c>
-      <c r="B53" t="s">
-        <v>120</v>
-      </c>
-      <c r="C53" t="s">
-        <v>246</v>
-      </c>
-      <c r="D53" t="s">
-        <v>415</v>
-      </c>
-      <c r="E53" t="s">
-        <v>105</v>
-      </c>
-      <c r="F53" t="s">
-        <v>268</v>
-      </c>
-      <c r="G53" t="s">
-        <v>309</v>
-      </c>
-      <c r="H53">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>38</v>
-      </c>
-      <c r="B54" t="s">
-        <v>39</v>
-      </c>
-      <c r="C54" t="s">
-        <v>781</v>
-      </c>
-      <c r="D54" t="s">
-        <v>412</v>
-      </c>
-      <c r="E54" t="s">
-        <v>731</v>
-      </c>
-      <c r="F54" t="s">
-        <v>303</v>
-      </c>
-      <c r="G54" t="s">
-        <v>311</v>
-      </c>
-      <c r="H54">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>45</v>
-      </c>
-      <c r="B55" t="s">
-        <v>46</v>
-      </c>
-      <c r="C55" t="s">
-        <v>782</v>
-      </c>
-      <c r="D55" t="s">
-        <v>412</v>
-      </c>
-      <c r="E55" t="s">
-        <v>47</v>
-      </c>
-      <c r="F55" t="s">
-        <v>318</v>
-      </c>
-      <c r="G55" t="s">
-        <v>318</v>
-      </c>
-      <c r="H55">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>34</v>
-      </c>
-      <c r="B56" t="s">
-        <v>35</v>
-      </c>
-      <c r="C56" t="s">
-        <v>783</v>
-      </c>
-      <c r="D56" t="s">
-        <v>415</v>
-      </c>
-      <c r="E56" t="s">
-        <v>36</v>
-      </c>
-      <c r="F56" t="s">
-        <v>303</v>
-      </c>
-      <c r="G56" t="s">
-        <v>255</v>
-      </c>
-      <c r="H56">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>381</v>
-      </c>
-      <c r="B57" t="s">
-        <v>382</v>
-      </c>
-      <c r="C57" t="s">
-        <v>791</v>
-      </c>
-      <c r="D57" t="s">
-        <v>414</v>
-      </c>
-      <c r="E57" t="s">
-        <v>383</v>
-      </c>
-      <c r="F57" t="s">
-        <v>303</v>
-      </c>
-      <c r="G57" t="s">
-        <v>303</v>
-      </c>
-      <c r="H57">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>737</v>
-      </c>
-      <c r="B58" t="s">
-        <v>738</v>
-      </c>
-      <c r="C58" t="s">
-        <v>792</v>
-      </c>
-      <c r="D58" t="s">
-        <v>414</v>
-      </c>
-      <c r="E58" t="s">
-        <v>739</v>
-      </c>
-      <c r="F58" t="s">
-        <v>294</v>
-      </c>
-      <c r="G58" t="s">
-        <v>307</v>
-      </c>
-      <c r="H58">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>784</v>
-      </c>
-      <c r="B59" t="s">
-        <v>785</v>
-      </c>
-      <c r="C59" t="s">
-        <v>793</v>
-      </c>
-      <c r="D59" t="s">
-        <v>413</v>
-      </c>
-      <c r="E59" t="s">
-        <v>786</v>
-      </c>
-      <c r="F59" t="s">
-        <v>787</v>
-      </c>
-      <c r="G59" t="s">
-        <v>787</v>
-      </c>
-      <c r="H59">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>788</v>
-      </c>
-      <c r="B60" t="s">
-        <v>789</v>
-      </c>
-      <c r="C60" t="s">
-        <v>794</v>
-      </c>
-      <c r="D60" t="s">
-        <v>414</v>
-      </c>
-      <c r="E60" t="s">
-        <v>790</v>
-      </c>
-      <c r="F60" t="s">
-        <v>324</v>
-      </c>
-      <c r="H60">
+      <c r="E60">
         <v>1</v>
       </c>
     </row>
@@ -11207,10 +10517,10 @@
         <v>2</v>
       </c>
       <c r="C69" s="24" t="s">
-        <v>784</v>
+        <v>740</v>
       </c>
       <c r="D69" s="25" t="s">
-        <v>785</v>
+        <v>741</v>
       </c>
       <c r="E69" s="24">
         <v>6103064219</v>
@@ -11220,7 +10530,7 @@
         <v>610-306-4219</v>
       </c>
       <c r="G69" s="24" t="s">
-        <v>786</v>
+        <v>742</v>
       </c>
       <c r="H69" s="24" t="str">
         <f>_xlfn.CONCAT(G69,","," College Park MD")</f>
@@ -11272,10 +10582,10 @@
         <v>3</v>
       </c>
       <c r="C70" s="24" t="s">
-        <v>788</v>
+        <v>744</v>
       </c>
       <c r="D70" s="25" t="s">
-        <v>789</v>
+        <v>745</v>
       </c>
       <c r="E70" s="24">
         <v>3017424442</v>
@@ -11285,7 +10595,7 @@
         <v>301-742-4442</v>
       </c>
       <c r="G70" s="24" t="s">
-        <v>790</v>
+        <v>746</v>
       </c>
       <c r="H70" s="24" t="str">
         <f>_xlfn.CONCAT(G70,","," College Park MD")</f>

</xml_diff>